<commit_message>
chore(update) for 21/11/2025 - update master to laters version - update cekunit report to laters version - and update sp sender to lates version on date 18 jto
</commit_message>
<xml_diff>
--- a/src/sp/LAPORAN SP DIGITIAL BULAN NOVEMBER 2025.xlsx
+++ b/src/sp/LAPORAN SP DIGITIAL BULAN NOVEMBER 2025.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7275" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7275" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="14-11-25" sheetId="1" r:id="rId1"/>
     <sheet name="15-11-25" sheetId="2" r:id="rId2"/>
     <sheet name="16-11-25" sheetId="3" r:id="rId3"/>
     <sheet name="17-11-25" sheetId="4" r:id="rId4"/>
+    <sheet name="18-11-25" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'16-11-25'!$J$5:$L$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'14-11-25'!$J$5:$L$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'15-11-25'!$A$4:$H$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'18-11-25'!$A$4:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="885">
   <si>
     <t>LAPORAN SP DIGITAL BULAN NOVEMBER 2025</t>
   </si>
@@ -2306,6 +2308,390 @@
   </si>
   <si>
     <t>082387285974</t>
+  </si>
+  <si>
+    <t>TP-25-F0000447</t>
+  </si>
+  <si>
+    <t>AGUS WANASIR</t>
+  </si>
+  <si>
+    <t>082288221744</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SP-25-F0000397</t>
+  </si>
+  <si>
+    <t>ANTONIUS GINTING</t>
+  </si>
+  <si>
+    <t>081270039201</t>
+  </si>
+  <si>
+    <t>TP-24-F0000717</t>
+  </si>
+  <si>
+    <t>BARTOLOMIUS BOLI IKEN</t>
+  </si>
+  <si>
+    <t>082391314216</t>
+  </si>
+  <si>
+    <t>SP-25-F0002615</t>
+  </si>
+  <si>
+    <t>BONEFASIUS RESI</t>
+  </si>
+  <si>
+    <t>087815962429</t>
+  </si>
+  <si>
+    <t>OD-24-F0001344</t>
+  </si>
+  <si>
+    <t>BUDI SANTOSO</t>
+  </si>
+  <si>
+    <t>0895362793339</t>
+  </si>
+  <si>
+    <t>TP-25-F0000161</t>
+  </si>
+  <si>
+    <t>CHODI HERNANDA</t>
+  </si>
+  <si>
+    <t>083841794043</t>
+  </si>
+  <si>
+    <t>OD-25-F0000183</t>
+  </si>
+  <si>
+    <t>DESI HANDAYANI</t>
+  </si>
+  <si>
+    <t>082174008931</t>
+  </si>
+  <si>
+    <t>SP-23-F0001469</t>
+  </si>
+  <si>
+    <t>DESSY SUSANTY</t>
+  </si>
+  <si>
+    <t>082172005095</t>
+  </si>
+  <si>
+    <t>SP-25-F0000153</t>
+  </si>
+  <si>
+    <t>FEBRI SAPUTRA</t>
+  </si>
+  <si>
+    <t>085364444718</t>
+  </si>
+  <si>
+    <t>SP-24-F0001227</t>
+  </si>
+  <si>
+    <t>HAMDANI ZALUKHU</t>
+  </si>
+  <si>
+    <t>082169861118</t>
+  </si>
+  <si>
+    <t>OD-25-F0001862</t>
+  </si>
+  <si>
+    <t>HARIS</t>
+  </si>
+  <si>
+    <t>085709454246</t>
+  </si>
+  <si>
+    <t>OD-24-F0003473</t>
+  </si>
+  <si>
+    <t>IQBAL RAMADHAN</t>
+  </si>
+  <si>
+    <t>081276553866</t>
+  </si>
+  <si>
+    <t>SP-24-F0002220</t>
+  </si>
+  <si>
+    <t>ISTINGADAH</t>
+  </si>
+  <si>
+    <t>081336445554</t>
+  </si>
+  <si>
+    <t>TP-25-F0000518</t>
+  </si>
+  <si>
+    <t>IWAN KURNIAWAN</t>
+  </si>
+  <si>
+    <t>081388381424</t>
+  </si>
+  <si>
+    <t>SP-25-F0001418</t>
+  </si>
+  <si>
+    <t>JUKRI</t>
+  </si>
+  <si>
+    <t>085935371564</t>
+  </si>
+  <si>
+    <t>SP-24-F0000984</t>
+  </si>
+  <si>
+    <t>JUMARNO</t>
+  </si>
+  <si>
+    <t>081276300886</t>
+  </si>
+  <si>
+    <t>SP-25-F0002614</t>
+  </si>
+  <si>
+    <t>KARNO NUGROHO</t>
+  </si>
+  <si>
+    <t>081915810018</t>
+  </si>
+  <si>
+    <t>TP-24-F0000806</t>
+  </si>
+  <si>
+    <t>KATMINAH</t>
+  </si>
+  <si>
+    <t>082285616369</t>
+  </si>
+  <si>
+    <t>OD-25-F0000479</t>
+  </si>
+  <si>
+    <t>MASDARIONO SIHOTANG</t>
+  </si>
+  <si>
+    <t>082170550097</t>
+  </si>
+  <si>
+    <t>TP-24-F0000380</t>
+  </si>
+  <si>
+    <t>MOHAMAD PARKUSNADI</t>
+  </si>
+  <si>
+    <t>081226431642</t>
+  </si>
+  <si>
+    <t>SP-25-F0000642</t>
+  </si>
+  <si>
+    <t>MUDIN DAULAY</t>
+  </si>
+  <si>
+    <t>085359128799</t>
+  </si>
+  <si>
+    <t>OD-25-F0001224</t>
+  </si>
+  <si>
+    <t>MUH. SYAIMURI</t>
+  </si>
+  <si>
+    <t>082169082092</t>
+  </si>
+  <si>
+    <t>TP-24-F0000714</t>
+  </si>
+  <si>
+    <t>MUHAMAD ALFIANSAH</t>
+  </si>
+  <si>
+    <t>083165012773</t>
+  </si>
+  <si>
+    <t>SP-24-F0000995</t>
+  </si>
+  <si>
+    <t>MUHAMMAD DAHLAN LUBIS</t>
+  </si>
+  <si>
+    <t>081915817992</t>
+  </si>
+  <si>
+    <t>SP-25-F0001409</t>
+  </si>
+  <si>
+    <t>NIKO DEMUS TAMBUNAN</t>
+  </si>
+  <si>
+    <t>081261350004</t>
+  </si>
+  <si>
+    <t>TP-24-F0000023</t>
+  </si>
+  <si>
+    <t>NOVITA ASTUTI</t>
+  </si>
+  <si>
+    <t>082283212592</t>
+  </si>
+  <si>
+    <t>SP-24-F0002217</t>
+  </si>
+  <si>
+    <t>RAFI FAIQAL MUSFAR</t>
+  </si>
+  <si>
+    <t>080602425552</t>
+  </si>
+  <si>
+    <t>OD-25-F0001735</t>
+  </si>
+  <si>
+    <t>RAJA MUHD ZAHARI</t>
+  </si>
+  <si>
+    <t>087753663661</t>
+  </si>
+  <si>
+    <t>OD-24-F0001655</t>
+  </si>
+  <si>
+    <t>RATNA PERTIWI</t>
+  </si>
+  <si>
+    <t>081275903611</t>
+  </si>
+  <si>
+    <t>TP-25-F0000061</t>
+  </si>
+  <si>
+    <t>RIKI SETIAWAN</t>
+  </si>
+  <si>
+    <t>081268098518</t>
+  </si>
+  <si>
+    <t>OD-25-F0001705</t>
+  </si>
+  <si>
+    <t>RIO SYAHPUTRA SILALAHI</t>
+  </si>
+  <si>
+    <t>085274300556</t>
+  </si>
+  <si>
+    <t>SP-24-F0001223</t>
+  </si>
+  <si>
+    <t>RULY PUJI ASTUTIK</t>
+  </si>
+  <si>
+    <t>082171394706</t>
+  </si>
+  <si>
+    <t>TP-25-F0000516</t>
+  </si>
+  <si>
+    <t>RUSWANDI</t>
+  </si>
+  <si>
+    <t>083809537525</t>
+  </si>
+  <si>
+    <t>OD-23-F0001592</t>
+  </si>
+  <si>
+    <t>RYAS DWI SETIANINGRUM</t>
+  </si>
+  <si>
+    <t>085230180471</t>
+  </si>
+  <si>
+    <t>SP-25-F0001419</t>
+  </si>
+  <si>
+    <t>SAMINI MINDASARI</t>
+  </si>
+  <si>
+    <t>083198153405</t>
+  </si>
+  <si>
+    <t>TERIKIRIM CENTANG 1</t>
+  </si>
+  <si>
+    <t>TP-24-F0000809</t>
+  </si>
+  <si>
+    <t>SAPRUDIN</t>
+  </si>
+  <si>
+    <t>089668009848</t>
+  </si>
+  <si>
+    <t>TP-24-F0000805</t>
+  </si>
+  <si>
+    <t>SEFRI KURNIAWAN</t>
+  </si>
+  <si>
+    <t>081364363605</t>
+  </si>
+  <si>
+    <t>TP-25-F0000586</t>
+  </si>
+  <si>
+    <t>SHAKTI WICAKSANA</t>
+  </si>
+  <si>
+    <t>082390506353</t>
+  </si>
+  <si>
+    <t>OD-25-F0000180</t>
+  </si>
+  <si>
+    <t>SUPADI</t>
+  </si>
+  <si>
+    <t>082185598061</t>
+  </si>
+  <si>
+    <t>SP-24-F0001467</t>
+  </si>
+  <si>
+    <t>WAHYU NUR ZUBAIDAH</t>
+  </si>
+  <si>
+    <t>085669007231</t>
+  </si>
+  <si>
+    <t>OD-24-F0001645</t>
+  </si>
+  <si>
+    <t>WARDAM</t>
+  </si>
+  <si>
+    <t>082170801284</t>
+  </si>
+  <si>
+    <t>OD-25-F0001708</t>
+  </si>
+  <si>
+    <t>WIRANTO</t>
+  </si>
+  <si>
+    <t>08117713008</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2704,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2336,13 +2722,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2494,7 +2873,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2582,12 +2961,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2851,28 +3224,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2881,118 +3257,115 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3003,8 +3376,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -5697,7 +6070,7 @@
       <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -5764,7 +6137,7 @@
       <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -6247,7 +6620,7 @@
       <c r="G27" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -6282,7 +6655,7 @@
       <c r="G28" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -6413,7 +6786,7 @@
       <c r="G32" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -6541,20 +6914,20 @@
       <c r="F36" t="s">
         <v>298</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="K36" s="4" t="str">
+      <c r="K36" s="5" t="str">
         <f t="shared" si="1"/>
         <v>088279723233</v>
       </c>
-      <c r="L36" s="4" t="str">
+      <c r="L36" s="5" t="str">
         <f t="shared" si="2"/>
         <v>JOHANNA BASARIA TOBING</v>
       </c>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
@@ -8393,7 +8766,7 @@
       <c r="H6" s="3">
         <v>45980</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="5">
         <f t="shared" ref="J6:J64" si="0">A6</f>
         <v>2</v>
       </c>
@@ -8638,7 +9011,7 @@
       <c r="H13" s="3">
         <v>45980</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -8778,7 +9151,7 @@
       <c r="H17" s="3">
         <v>45980</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -8813,7 +9186,7 @@
       <c r="H18" s="3">
         <v>45980</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -8848,7 +9221,7 @@
       <c r="H19" s="3">
         <v>45980</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -8918,7 +9291,7 @@
       <c r="H21" s="3">
         <v>45980</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -10456,8 +10829,8 @@
   <sheetPr/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -10559,7 +10932,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>22921</v>
+        <v>22821</v>
       </c>
       <c r="C6" t="s">
         <v>640</v>
@@ -10594,7 +10967,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>23022</v>
+        <v>22822</v>
       </c>
       <c r="C7" t="s">
         <v>643</v>
@@ -10629,7 +11002,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>23123</v>
+        <v>22823</v>
       </c>
       <c r="C8" t="s">
         <v>646</v>
@@ -10664,7 +11037,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>23224</v>
+        <v>22824</v>
       </c>
       <c r="C9" t="s">
         <v>649</v>
@@ -10699,7 +11072,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>23325</v>
+        <v>22825</v>
       </c>
       <c r="C10" t="s">
         <v>652</v>
@@ -10734,7 +11107,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>23426</v>
+        <v>22826</v>
       </c>
       <c r="C11" t="s">
         <v>655</v>
@@ -10769,7 +11142,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>23527</v>
+        <v>22827</v>
       </c>
       <c r="C12" t="s">
         <v>658</v>
@@ -10804,7 +11177,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>23628</v>
+        <v>22828</v>
       </c>
       <c r="C13" t="s">
         <v>661</v>
@@ -10839,7 +11212,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>23729</v>
+        <v>22829</v>
       </c>
       <c r="C14" t="s">
         <v>664</v>
@@ -10874,7 +11247,7 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>23830</v>
+        <v>22830</v>
       </c>
       <c r="C15" t="s">
         <v>667</v>
@@ -10909,7 +11282,7 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>23931</v>
+        <v>22831</v>
       </c>
       <c r="C16" t="s">
         <v>670</v>
@@ -10944,7 +11317,7 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>24032</v>
+        <v>22832</v>
       </c>
       <c r="C17" t="s">
         <v>673</v>
@@ -10979,7 +11352,7 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <v>24133</v>
+        <v>22833</v>
       </c>
       <c r="C18" t="s">
         <v>676</v>
@@ -11014,7 +11387,7 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <v>24234</v>
+        <v>22834</v>
       </c>
       <c r="C19" t="s">
         <v>679</v>
@@ -11049,7 +11422,7 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <v>24335</v>
+        <v>22835</v>
       </c>
       <c r="C20" t="s">
         <v>682</v>
@@ -11084,7 +11457,7 @@
         <v>17</v>
       </c>
       <c r="B21">
-        <v>24436</v>
+        <v>22836</v>
       </c>
       <c r="C21" t="s">
         <v>685</v>
@@ -11119,7 +11492,7 @@
         <v>18</v>
       </c>
       <c r="B22">
-        <v>24537</v>
+        <v>22837</v>
       </c>
       <c r="C22" t="s">
         <v>688</v>
@@ -11154,7 +11527,7 @@
         <v>19</v>
       </c>
       <c r="B23">
-        <v>24638</v>
+        <v>22838</v>
       </c>
       <c r="C23" t="s">
         <v>691</v>
@@ -11189,7 +11562,7 @@
         <v>20</v>
       </c>
       <c r="B24">
-        <v>24739</v>
+        <v>22839</v>
       </c>
       <c r="C24" t="s">
         <v>694</v>
@@ -11224,7 +11597,7 @@
         <v>21</v>
       </c>
       <c r="B25">
-        <v>24840</v>
+        <v>22840</v>
       </c>
       <c r="C25" t="s">
         <v>697</v>
@@ -11259,7 +11632,7 @@
         <v>22</v>
       </c>
       <c r="B26">
-        <v>24941</v>
+        <v>22841</v>
       </c>
       <c r="C26" t="s">
         <v>700</v>
@@ -11294,7 +11667,7 @@
         <v>23</v>
       </c>
       <c r="B27">
-        <v>25042</v>
+        <v>22842</v>
       </c>
       <c r="C27" t="s">
         <v>703</v>
@@ -11329,7 +11702,7 @@
         <v>24</v>
       </c>
       <c r="B28">
-        <v>25143</v>
+        <v>22843</v>
       </c>
       <c r="C28" t="s">
         <v>706</v>
@@ -11364,7 +11737,7 @@
         <v>25</v>
       </c>
       <c r="B29">
-        <v>25244</v>
+        <v>22844</v>
       </c>
       <c r="C29" t="s">
         <v>709</v>
@@ -11399,7 +11772,7 @@
         <v>26</v>
       </c>
       <c r="B30">
-        <v>25345</v>
+        <v>22845</v>
       </c>
       <c r="C30" t="s">
         <v>712</v>
@@ -11434,7 +11807,7 @@
         <v>27</v>
       </c>
       <c r="B31">
-        <v>25446</v>
+        <v>22846</v>
       </c>
       <c r="C31" t="s">
         <v>715</v>
@@ -11469,7 +11842,7 @@
         <v>28</v>
       </c>
       <c r="B32">
-        <v>25547</v>
+        <v>22847</v>
       </c>
       <c r="C32" t="s">
         <v>718</v>
@@ -11504,7 +11877,7 @@
         <v>29</v>
       </c>
       <c r="B33">
-        <v>25648</v>
+        <v>22848</v>
       </c>
       <c r="C33" t="s">
         <v>721</v>
@@ -11539,7 +11912,7 @@
         <v>30</v>
       </c>
       <c r="B34">
-        <v>25749</v>
+        <v>22849</v>
       </c>
       <c r="C34" t="s">
         <v>724</v>
@@ -11574,7 +11947,7 @@
         <v>31</v>
       </c>
       <c r="B35">
-        <v>25850</v>
+        <v>22850</v>
       </c>
       <c r="C35" t="s">
         <v>727</v>
@@ -11609,7 +11982,7 @@
         <v>32</v>
       </c>
       <c r="B36">
-        <v>25951</v>
+        <v>22851</v>
       </c>
       <c r="C36" t="s">
         <v>730</v>
@@ -11644,7 +12017,7 @@
         <v>33</v>
       </c>
       <c r="B37">
-        <v>26052</v>
+        <v>22852</v>
       </c>
       <c r="C37" t="s">
         <v>733</v>
@@ -11679,7 +12052,7 @@
         <v>34</v>
       </c>
       <c r="B38">
-        <v>26153</v>
+        <v>22853</v>
       </c>
       <c r="C38" t="s">
         <v>736</v>
@@ -11714,7 +12087,7 @@
         <v>35</v>
       </c>
       <c r="B39">
-        <v>26254</v>
+        <v>22854</v>
       </c>
       <c r="C39" t="s">
         <v>739</v>
@@ -11749,7 +12122,7 @@
         <v>36</v>
       </c>
       <c r="B40">
-        <v>26355</v>
+        <v>22855</v>
       </c>
       <c r="C40" t="s">
         <v>742</v>
@@ -11784,7 +12157,7 @@
         <v>37</v>
       </c>
       <c r="B41">
-        <v>26456</v>
+        <v>22856</v>
       </c>
       <c r="C41" t="s">
         <v>745</v>
@@ -11819,7 +12192,7 @@
         <v>38</v>
       </c>
       <c r="B42">
-        <v>26557</v>
+        <v>22857</v>
       </c>
       <c r="C42" t="s">
         <v>748</v>
@@ -11854,7 +12227,7 @@
         <v>39</v>
       </c>
       <c r="B43">
-        <v>26658</v>
+        <v>22858</v>
       </c>
       <c r="C43" t="s">
         <v>751</v>
@@ -11889,7 +12262,7 @@
         <v>40</v>
       </c>
       <c r="B44">
-        <v>26759</v>
+        <v>22859</v>
       </c>
       <c r="C44" t="s">
         <v>754</v>
@@ -11929,4 +12302,1684 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.57142857142857" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="16.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="28.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="4.71428571428571" customWidth="1"/>
+    <col min="6" max="6" width="15.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="22.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="16.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="3.57142857142857" customWidth="1"/>
+    <col min="11" max="11" width="15.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="28.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>22820</v>
+      </c>
+      <c r="C5" t="s">
+        <v>757</v>
+      </c>
+      <c r="D5" t="s">
+        <v>758</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>759</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>760</v>
+      </c>
+      <c r="J5">
+        <f>A5</f>
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
+        <f>F5</f>
+        <v>082288221744</v>
+      </c>
+      <c r="L5" t="str">
+        <f>D5</f>
+        <v>AGUS WANASIR</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>22821</v>
+      </c>
+      <c r="C6" t="s">
+        <v>761</v>
+      </c>
+      <c r="D6" t="s">
+        <v>762</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>763</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J46" si="0">A6</f>
+        <v>2</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K46" si="1">F6</f>
+        <v>081270039201</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L46" si="2">D6</f>
+        <v>ANTONIUS GINTING</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>22822</v>
+      </c>
+      <c r="C7" t="s">
+        <v>764</v>
+      </c>
+      <c r="D7" t="s">
+        <v>765</v>
+      </c>
+      <c r="E7">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>766</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>082391314216</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>BARTOLOMIUS BOLI IKEN</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>22823</v>
+      </c>
+      <c r="C8" t="s">
+        <v>767</v>
+      </c>
+      <c r="D8" t="s">
+        <v>768</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>769</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>087815962429</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>BONEFASIUS RESI</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>22824</v>
+      </c>
+      <c r="C9" t="s">
+        <v>770</v>
+      </c>
+      <c r="D9" t="s">
+        <v>771</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>772</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>0895362793339</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>BUDI SANTOSO</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>22825</v>
+      </c>
+      <c r="C10" t="s">
+        <v>773</v>
+      </c>
+      <c r="D10" t="s">
+        <v>774</v>
+      </c>
+      <c r="E10">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>775</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>083841794043</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>CHODI HERNANDA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>22826</v>
+      </c>
+      <c r="C11" t="s">
+        <v>776</v>
+      </c>
+      <c r="D11" t="s">
+        <v>777</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>778</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>082174008931</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>DESI HANDAYANI</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>22827</v>
+      </c>
+      <c r="C12" t="s">
+        <v>779</v>
+      </c>
+      <c r="D12" t="s">
+        <v>780</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>781</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>082172005095</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>DESSY SUSANTY</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>22828</v>
+      </c>
+      <c r="C13" t="s">
+        <v>782</v>
+      </c>
+      <c r="D13" t="s">
+        <v>783</v>
+      </c>
+      <c r="E13">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>784</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>085364444718</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>FEBRI SAPUTRA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>22829</v>
+      </c>
+      <c r="C14" t="s">
+        <v>785</v>
+      </c>
+      <c r="D14" t="s">
+        <v>786</v>
+      </c>
+      <c r="E14">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>787</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>082169861118</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>HAMDANI ZALUKHU</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>22830</v>
+      </c>
+      <c r="C15" t="s">
+        <v>788</v>
+      </c>
+      <c r="D15" t="s">
+        <v>789</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>790</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>085709454246</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>HARIS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>22831</v>
+      </c>
+      <c r="C16" t="s">
+        <v>791</v>
+      </c>
+      <c r="D16" t="s">
+        <v>792</v>
+      </c>
+      <c r="E16">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>793</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>081276553866</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>IQBAL RAMADHAN</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>22832</v>
+      </c>
+      <c r="C17" t="s">
+        <v>794</v>
+      </c>
+      <c r="D17" t="s">
+        <v>795</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>796</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>081336445554</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>ISTINGADAH</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>22833</v>
+      </c>
+      <c r="C18" t="s">
+        <v>797</v>
+      </c>
+      <c r="D18" t="s">
+        <v>798</v>
+      </c>
+      <c r="E18">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>799</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>081388381424</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>IWAN KURNIAWAN</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>22834</v>
+      </c>
+      <c r="C19" t="s">
+        <v>800</v>
+      </c>
+      <c r="D19" t="s">
+        <v>801</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>802</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>085935371564</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>JUKRI</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>22835</v>
+      </c>
+      <c r="C20" t="s">
+        <v>803</v>
+      </c>
+      <c r="D20" t="s">
+        <v>804</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>805</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>081276300886</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>JUMARNO</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>22836</v>
+      </c>
+      <c r="C21" t="s">
+        <v>806</v>
+      </c>
+      <c r="D21" t="s">
+        <v>807</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>808</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>081915810018</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>KARNO NUGROHO</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>22837</v>
+      </c>
+      <c r="C22" t="s">
+        <v>809</v>
+      </c>
+      <c r="D22" t="s">
+        <v>810</v>
+      </c>
+      <c r="E22">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>811</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>760</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>082285616369</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>KATMINAH</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>22838</v>
+      </c>
+      <c r="C23" t="s">
+        <v>812</v>
+      </c>
+      <c r="D23" t="s">
+        <v>813</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>814</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>760</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>082170550097</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="2"/>
+        <v>MASDARIONO SIHOTANG</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>22839</v>
+      </c>
+      <c r="C24" t="s">
+        <v>815</v>
+      </c>
+      <c r="D24" t="s">
+        <v>816</v>
+      </c>
+      <c r="E24">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>817</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>760</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>081226431642</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="2"/>
+        <v>MOHAMAD PARKUSNADI</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>22840</v>
+      </c>
+      <c r="C25" t="s">
+        <v>818</v>
+      </c>
+      <c r="D25" t="s">
+        <v>819</v>
+      </c>
+      <c r="E25">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>820</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>085359128799</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="2"/>
+        <v>MUDIN DAULAY</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>22841</v>
+      </c>
+      <c r="C26" t="s">
+        <v>821</v>
+      </c>
+      <c r="D26" t="s">
+        <v>822</v>
+      </c>
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>823</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>082169082092</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="2"/>
+        <v>MUH. SYAIMURI</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>22842</v>
+      </c>
+      <c r="C27" t="s">
+        <v>824</v>
+      </c>
+      <c r="D27" t="s">
+        <v>825</v>
+      </c>
+      <c r="E27">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>826</v>
+      </c>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>083165012773</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="2"/>
+        <v>MUHAMAD ALFIANSAH</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>22843</v>
+      </c>
+      <c r="C28" t="s">
+        <v>827</v>
+      </c>
+      <c r="D28" t="s">
+        <v>828</v>
+      </c>
+      <c r="E28">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>829</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>081915817992</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="2"/>
+        <v>MUHAMMAD DAHLAN LUBIS</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>22844</v>
+      </c>
+      <c r="C29" t="s">
+        <v>830</v>
+      </c>
+      <c r="D29" t="s">
+        <v>831</v>
+      </c>
+      <c r="E29">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>832</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>081261350004</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="2"/>
+        <v>NIKO DEMUS TAMBUNAN</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>22845</v>
+      </c>
+      <c r="C30" t="s">
+        <v>833</v>
+      </c>
+      <c r="D30" t="s">
+        <v>834</v>
+      </c>
+      <c r="E30">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>835</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>082283212592</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="2"/>
+        <v>NOVITA ASTUTI</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>22846</v>
+      </c>
+      <c r="C31" t="s">
+        <v>836</v>
+      </c>
+      <c r="D31" t="s">
+        <v>837</v>
+      </c>
+      <c r="E31">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>838</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>760</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>080602425552</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="2"/>
+        <v>RAFI FAIQAL MUSFAR</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>22847</v>
+      </c>
+      <c r="C32" t="s">
+        <v>839</v>
+      </c>
+      <c r="D32" t="s">
+        <v>840</v>
+      </c>
+      <c r="E32">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>841</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>087753663661</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="2"/>
+        <v>RAJA MUHD ZAHARI</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>22848</v>
+      </c>
+      <c r="C33" t="s">
+        <v>842</v>
+      </c>
+      <c r="D33" t="s">
+        <v>843</v>
+      </c>
+      <c r="E33">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>844</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>081275903611</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="2"/>
+        <v>RATNA PERTIWI</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>22849</v>
+      </c>
+      <c r="C34" t="s">
+        <v>845</v>
+      </c>
+      <c r="D34" t="s">
+        <v>846</v>
+      </c>
+      <c r="E34">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>847</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>081268098518</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="2"/>
+        <v>RIKI SETIAWAN</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>22850</v>
+      </c>
+      <c r="C35" t="s">
+        <v>848</v>
+      </c>
+      <c r="D35" t="s">
+        <v>849</v>
+      </c>
+      <c r="E35">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>850</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>760</v>
+      </c>
+      <c r="J35" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>085274300556</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="2"/>
+        <v>RIO SYAHPUTRA SILALAHI</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>22851</v>
+      </c>
+      <c r="C36" t="s">
+        <v>851</v>
+      </c>
+      <c r="D36" t="s">
+        <v>852</v>
+      </c>
+      <c r="E36">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>853</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>760</v>
+      </c>
+      <c r="J36" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>082171394706</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="2"/>
+        <v>RULY PUJI ASTUTIK</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>22852</v>
+      </c>
+      <c r="C37" t="s">
+        <v>854</v>
+      </c>
+      <c r="D37" t="s">
+        <v>855</v>
+      </c>
+      <c r="E37">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>856</v>
+      </c>
+      <c r="G37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>083809537525</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="2"/>
+        <v>RUSWANDI</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>22853</v>
+      </c>
+      <c r="C38" t="s">
+        <v>857</v>
+      </c>
+      <c r="D38" t="s">
+        <v>858</v>
+      </c>
+      <c r="E38">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>859</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>085230180471</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="2"/>
+        <v>RYAS DWI SETIANINGRUM</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>22854</v>
+      </c>
+      <c r="C39" t="s">
+        <v>860</v>
+      </c>
+      <c r="D39" t="s">
+        <v>861</v>
+      </c>
+      <c r="E39">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>862</v>
+      </c>
+      <c r="G39" t="s">
+        <v>863</v>
+      </c>
+      <c r="H39" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>083198153405</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="2"/>
+        <v>SAMINI MINDASARI</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>22855</v>
+      </c>
+      <c r="C40" t="s">
+        <v>864</v>
+      </c>
+      <c r="D40" t="s">
+        <v>865</v>
+      </c>
+      <c r="E40">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>866</v>
+      </c>
+      <c r="G40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>089668009848</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="2"/>
+        <v>SAPRUDIN</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>22856</v>
+      </c>
+      <c r="C41" t="s">
+        <v>867</v>
+      </c>
+      <c r="D41" t="s">
+        <v>868</v>
+      </c>
+      <c r="E41">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>869</v>
+      </c>
+      <c r="G41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>081364363605</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="2"/>
+        <v>SEFRI KURNIAWAN</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>22857</v>
+      </c>
+      <c r="C42" t="s">
+        <v>870</v>
+      </c>
+      <c r="D42" t="s">
+        <v>871</v>
+      </c>
+      <c r="E42">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>872</v>
+      </c>
+      <c r="G42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>082390506353</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="2"/>
+        <v>SHAKTI WICAKSANA</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>22858</v>
+      </c>
+      <c r="C43" t="s">
+        <v>873</v>
+      </c>
+      <c r="D43" t="s">
+        <v>874</v>
+      </c>
+      <c r="E43">
+        <v>18</v>
+      </c>
+      <c r="F43" t="s">
+        <v>875</v>
+      </c>
+      <c r="G43" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>082185598061</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="2"/>
+        <v>SUPADI</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>22859</v>
+      </c>
+      <c r="C44" t="s">
+        <v>876</v>
+      </c>
+      <c r="D44" t="s">
+        <v>877</v>
+      </c>
+      <c r="E44">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>878</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="3">
+        <v>45982</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>085669007231</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="2"/>
+        <v>WAHYU NUR ZUBAIDAH</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>22860</v>
+      </c>
+      <c r="C45" t="s">
+        <v>879</v>
+      </c>
+      <c r="D45" t="s">
+        <v>880</v>
+      </c>
+      <c r="E45">
+        <v>18</v>
+      </c>
+      <c r="F45" t="s">
+        <v>881</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>760</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>082170801284</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="2"/>
+        <v>WARDAM</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>22861</v>
+      </c>
+      <c r="C46" t="s">
+        <v>882</v>
+      </c>
+      <c r="D46" t="s">
+        <v>883</v>
+      </c>
+      <c r="E46">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>884</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" t="s">
+        <v>760</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>08117713008</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="2"/>
+        <v>WIRANTO</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A5:H46">
+    <sortCondition ref="D5"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
master and daily reoport
</commit_message>
<xml_diff>
--- a/src/sp/LAPORAN SP DIGITIAL BULAN NOVEMBER 2025.xlsx
+++ b/src/sp/LAPORAN SP DIGITIAL BULAN NOVEMBER 2025.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7275" activeTab="4"/>
+    <workbookView windowWidth="20490" windowHeight="7275" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="14-11-25" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,11 @@
     <sheet name="16-11-25" sheetId="3" r:id="rId3"/>
     <sheet name="17-11-25" sheetId="4" r:id="rId4"/>
     <sheet name="18-11-25" sheetId="5" r:id="rId5"/>
+    <sheet name="19-11-25" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'16-11-25'!$J$5:$L$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'19-11-25'!$A$4:$H$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'14-11-25'!$J$5:$L$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'15-11-25'!$A$4:$H$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'18-11-25'!$A$4:$H$46</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="1036">
   <si>
     <t>LAPORAN SP DIGITAL BULAN NOVEMBER 2025</t>
   </si>
@@ -2692,6 +2694,459 @@
   </si>
   <si>
     <t>08117713008</t>
+  </si>
+  <si>
+    <t>TANGGAL KIRIM</t>
+  </si>
+  <si>
+    <t>OD-24-F0001082</t>
+  </si>
+  <si>
+    <t>ADISTO PRASATYO</t>
+  </si>
+  <si>
+    <t>085263362906</t>
+  </si>
+  <si>
+    <t>SP-24-F0001727</t>
+  </si>
+  <si>
+    <t>AGUS HERI SANTOSO</t>
+  </si>
+  <si>
+    <t>08126876989</t>
+  </si>
+  <si>
+    <t>TP-24-F0000387</t>
+  </si>
+  <si>
+    <t>ALFIAN</t>
+  </si>
+  <si>
+    <t>085374291252</t>
+  </si>
+  <si>
+    <t>SP-24-F0002504</t>
+  </si>
+  <si>
+    <t>AMIZAR ZULMI NASUTION</t>
+  </si>
+  <si>
+    <t>081266055292</t>
+  </si>
+  <si>
+    <t>TERKIRIM CENTANG 2 BLUM DIBACA</t>
+  </si>
+  <si>
+    <t>OD-24-F0001662</t>
+  </si>
+  <si>
+    <t>ANDIKA BATRA SUKARYA</t>
+  </si>
+  <si>
+    <t>082283149719</t>
+  </si>
+  <si>
+    <t>TP-25-F0000520</t>
+  </si>
+  <si>
+    <t>ANDIKA PAMUNGKAS</t>
+  </si>
+  <si>
+    <t>083892354614</t>
+  </si>
+  <si>
+    <t>TP-23-F0000501</t>
+  </si>
+  <si>
+    <t>ANGGA ARDIANSYAH</t>
+  </si>
+  <si>
+    <t>083188852207</t>
+  </si>
+  <si>
+    <t>SP-25-F0002091</t>
+  </si>
+  <si>
+    <t>ANGGA WIDI SYAHPUTRA</t>
+  </si>
+  <si>
+    <t>0895400640694</t>
+  </si>
+  <si>
+    <t>OD-25-F0000515</t>
+  </si>
+  <si>
+    <t>AZWALI KHAIRI</t>
+  </si>
+  <si>
+    <t>085356301551</t>
+  </si>
+  <si>
+    <t>SP-24-F0002496</t>
+  </si>
+  <si>
+    <t>BASARI</t>
+  </si>
+  <si>
+    <t>085765279425</t>
+  </si>
+  <si>
+    <t>SP-25-F0001422</t>
+  </si>
+  <si>
+    <t>CANDRA MUDA</t>
+  </si>
+  <si>
+    <t>082247069508</t>
+  </si>
+  <si>
+    <t>SP-25-F0000857</t>
+  </si>
+  <si>
+    <t>DAFIT HELDI</t>
+  </si>
+  <si>
+    <t>081374446609</t>
+  </si>
+  <si>
+    <t>TP-24-F0000638</t>
+  </si>
+  <si>
+    <t>EPI KARINA</t>
+  </si>
+  <si>
+    <t>081223853171</t>
+  </si>
+  <si>
+    <t>SP-24-F0002230</t>
+  </si>
+  <si>
+    <t>ESTER BR PARDEDE</t>
+  </si>
+  <si>
+    <t>082384226483</t>
+  </si>
+  <si>
+    <t>SP-25-F0001423</t>
+  </si>
+  <si>
+    <t>FERTO ATAUPAH</t>
+  </si>
+  <si>
+    <t>087845627099</t>
+  </si>
+  <si>
+    <t>TERKIRIM CENTANG 1</t>
+  </si>
+  <si>
+    <t>SP-25-F0002081</t>
+  </si>
+  <si>
+    <t>GUSTI JUPRI ANDA MAULANA</t>
+  </si>
+  <si>
+    <t>082171582482</t>
+  </si>
+  <si>
+    <t>SP-25-F0001040</t>
+  </si>
+  <si>
+    <t>HEBRA LENDI</t>
+  </si>
+  <si>
+    <t>088708395531</t>
+  </si>
+  <si>
+    <t>SP-25-F0002363</t>
+  </si>
+  <si>
+    <t>HENI FARIDA</t>
+  </si>
+  <si>
+    <t>085717412709</t>
+  </si>
+  <si>
+    <t>SP-25-F0002297</t>
+  </si>
+  <si>
+    <t>HERI PRATAMA</t>
+  </si>
+  <si>
+    <t>087714822536</t>
+  </si>
+  <si>
+    <t>SP-25-F0001125</t>
+  </si>
+  <si>
+    <t>HERY JUNIANTO</t>
+  </si>
+  <si>
+    <t>081350740931</t>
+  </si>
+  <si>
+    <t>OD-24-F0001661</t>
+  </si>
+  <si>
+    <t>IRA TRISULA ARDYANTI</t>
+  </si>
+  <si>
+    <t>085831045258</t>
+  </si>
+  <si>
+    <t>OD-24-F0002681</t>
+  </si>
+  <si>
+    <t>087784857563</t>
+  </si>
+  <si>
+    <t>OD-24-F0002947</t>
+  </si>
+  <si>
+    <t>ISMAIL</t>
+  </si>
+  <si>
+    <t>083838917190</t>
+  </si>
+  <si>
+    <t>TP-25-F0000655</t>
+  </si>
+  <si>
+    <t>JAPRI</t>
+  </si>
+  <si>
+    <t>081270074533</t>
+  </si>
+  <si>
+    <t>OD-24-F0003211</t>
+  </si>
+  <si>
+    <t>JUPRIANTO</t>
+  </si>
+  <si>
+    <t>082177252459</t>
+  </si>
+  <si>
+    <t>TP-24-F0000552</t>
+  </si>
+  <si>
+    <t>LAURA SYAFIKHA PUTRI</t>
+  </si>
+  <si>
+    <t>083809783587</t>
+  </si>
+  <si>
+    <t>SP-25-F0002356</t>
+  </si>
+  <si>
+    <t>LESMAN LUMBANTORUAN</t>
+  </si>
+  <si>
+    <t>082122082309</t>
+  </si>
+  <si>
+    <t>SP-25-F0002085</t>
+  </si>
+  <si>
+    <t>LUHUT SITUMORANG</t>
+  </si>
+  <si>
+    <t>082286941927</t>
+  </si>
+  <si>
+    <t>TERKIRIM DIBACA DAN DI BALAS</t>
+  </si>
+  <si>
+    <t>OD-24-F0002903</t>
+  </si>
+  <si>
+    <t>MARDIAH</t>
+  </si>
+  <si>
+    <t>085809836590</t>
+  </si>
+  <si>
+    <t>TERKIRIM DIBACA BELUM DI BALAS</t>
+  </si>
+  <si>
+    <t>SP-25-F0001063</t>
+  </si>
+  <si>
+    <t>MUHAMMAD BUDI</t>
+  </si>
+  <si>
+    <t>083835723800</t>
+  </si>
+  <si>
+    <t>SP-25-F0001088</t>
+  </si>
+  <si>
+    <t>MUHAMMAD HARIYANTO</t>
+  </si>
+  <si>
+    <t>089668459090</t>
+  </si>
+  <si>
+    <t>SP-25-F0001344</t>
+  </si>
+  <si>
+    <t>MUHAMMAD JUNAIDI</t>
+  </si>
+  <si>
+    <t>082339861630</t>
+  </si>
+  <si>
+    <t>TP-24-F0000551</t>
+  </si>
+  <si>
+    <t>MUJI HARYANTO</t>
+  </si>
+  <si>
+    <t>081364059451</t>
+  </si>
+  <si>
+    <t>TP-25-F0000652</t>
+  </si>
+  <si>
+    <t>MUSLIMIN</t>
+  </si>
+  <si>
+    <t>082287796354</t>
+  </si>
+  <si>
+    <t>SP-25-F0002037</t>
+  </si>
+  <si>
+    <t>NOVEDI LAOLI</t>
+  </si>
+  <si>
+    <t>082214594160</t>
+  </si>
+  <si>
+    <t>SP-25-F0001740</t>
+  </si>
+  <si>
+    <t>POSMARITO NDRAHA</t>
+  </si>
+  <si>
+    <t>082294790044</t>
+  </si>
+  <si>
+    <t>OD-25-F0001578</t>
+  </si>
+  <si>
+    <t>RAFI RIZKY SYAHPUTRA</t>
+  </si>
+  <si>
+    <t>085769897824</t>
+  </si>
+  <si>
+    <t>OD-24-F0002950</t>
+  </si>
+  <si>
+    <t>RAHEL ANDRIANSYAH</t>
+  </si>
+  <si>
+    <t>088271719392</t>
+  </si>
+  <si>
+    <t>SP-24-F0002227</t>
+  </si>
+  <si>
+    <t>RIA SUHARTI</t>
+  </si>
+  <si>
+    <t>082172430974</t>
+  </si>
+  <si>
+    <t>TP-24-F0000640</t>
+  </si>
+  <si>
+    <t>RIAN ANGGARA SAPUTRA</t>
+  </si>
+  <si>
+    <t>082386778113</t>
+  </si>
+  <si>
+    <t>OD-25-F0001099</t>
+  </si>
+  <si>
+    <t>RIDWAN</t>
+  </si>
+  <si>
+    <t>081266670060</t>
+  </si>
+  <si>
+    <t>SP-24-F0002734</t>
+  </si>
+  <si>
+    <t>RINA SRI DEWI</t>
+  </si>
+  <si>
+    <t>087877303641</t>
+  </si>
+  <si>
+    <t>OD-25-F0001736</t>
+  </si>
+  <si>
+    <t>TARMIZI</t>
+  </si>
+  <si>
+    <t>6281374154280</t>
+  </si>
+  <si>
+    <t>OD-25-F0001738</t>
+  </si>
+  <si>
+    <t>TUMINI</t>
+  </si>
+  <si>
+    <t>085185741050</t>
+  </si>
+  <si>
+    <t>OD-25-F0001120</t>
+  </si>
+  <si>
+    <t>USMAN HADINATHA</t>
+  </si>
+  <si>
+    <t>081277441909</t>
+  </si>
+  <si>
+    <t>SP-24-F0002226</t>
+  </si>
+  <si>
+    <t>WENDRI</t>
+  </si>
+  <si>
+    <t>082351191910</t>
+  </si>
+  <si>
+    <t>SP-25-F0000411</t>
+  </si>
+  <si>
+    <t>YANTI</t>
+  </si>
+  <si>
+    <t>081365214431</t>
+  </si>
+  <si>
+    <t>SP-25-F0000409</t>
+  </si>
+  <si>
+    <t>YUNITA HANDAYANI</t>
+  </si>
+  <si>
+    <t>081371952939</t>
+  </si>
+  <si>
+    <t>TP-25-F0000228</t>
+  </si>
+  <si>
+    <t>ZATIAWATI</t>
+  </si>
+  <si>
+    <t>083824710553</t>
   </si>
 </sst>
 </file>
@@ -3375,8 +3830,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -8728,7 +9183,7 @@
       <c r="F5" t="s">
         <v>458</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>45980</v>
       </c>
       <c r="J5">
@@ -8763,7 +9218,7 @@
       <c r="F6" t="s">
         <v>461</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>45980</v>
       </c>
       <c r="J6" s="5">
@@ -8798,7 +9253,7 @@
       <c r="F7" t="s">
         <v>464</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>45980</v>
       </c>
       <c r="J7">
@@ -8833,7 +9288,7 @@
       <c r="F8" t="s">
         <v>467</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>45980</v>
       </c>
       <c r="J8">
@@ -8868,7 +9323,7 @@
       <c r="F9" t="s">
         <v>470</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>45980</v>
       </c>
       <c r="J9">
@@ -8903,7 +9358,7 @@
       <c r="F10" t="s">
         <v>473</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>45980</v>
       </c>
       <c r="J10">
@@ -8938,7 +9393,7 @@
       <c r="F11" t="s">
         <v>476</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>45980</v>
       </c>
       <c r="J11">
@@ -8973,7 +9428,7 @@
       <c r="F12" t="s">
         <v>479</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>45980</v>
       </c>
       <c r="J12">
@@ -9008,10 +9463,10 @@
       <c r="F13" t="s">
         <v>482</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>45980</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -9043,7 +9498,7 @@
       <c r="F14" t="s">
         <v>485</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>45980</v>
       </c>
       <c r="J14">
@@ -9078,7 +9533,7 @@
       <c r="F15" t="s">
         <v>488</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>45980</v>
       </c>
       <c r="J15">
@@ -9113,7 +9568,7 @@
       <c r="F16" t="s">
         <v>491</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>45980</v>
       </c>
       <c r="J16">
@@ -9148,10 +9603,10 @@
       <c r="F17" t="s">
         <v>494</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>45980</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -9183,10 +9638,10 @@
       <c r="F18" t="s">
         <v>497</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>45980</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -9218,7 +9673,7 @@
       <c r="F19" t="s">
         <v>500</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>45980</v>
       </c>
       <c r="J19" s="5">
@@ -9253,7 +9708,7 @@
       <c r="F20" t="s">
         <v>503</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>45980</v>
       </c>
       <c r="J20">
@@ -9288,7 +9743,7 @@
       <c r="F21" t="s">
         <v>506</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>45980</v>
       </c>
       <c r="J21" s="5">
@@ -9323,7 +9778,7 @@
       <c r="F22" t="s">
         <v>509</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>45980</v>
       </c>
       <c r="J22">
@@ -9358,7 +9813,7 @@
       <c r="F23" t="s">
         <v>512</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>45980</v>
       </c>
       <c r="J23">
@@ -9393,7 +9848,7 @@
       <c r="F24" t="s">
         <v>515</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>45980</v>
       </c>
       <c r="J24">
@@ -9428,7 +9883,7 @@
       <c r="F25" t="s">
         <v>518</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>45980</v>
       </c>
       <c r="J25">
@@ -9463,7 +9918,7 @@
       <c r="F26" t="s">
         <v>521</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>45980</v>
       </c>
       <c r="J26">
@@ -9498,7 +9953,7 @@
       <c r="F27" t="s">
         <v>524</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>45980</v>
       </c>
       <c r="J27">
@@ -9533,7 +9988,7 @@
       <c r="F28" t="s">
         <v>527</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>45980</v>
       </c>
       <c r="J28" s="6">
@@ -9568,7 +10023,7 @@
       <c r="F29" t="s">
         <v>530</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="4">
         <v>45980</v>
       </c>
       <c r="J29">
@@ -9603,7 +10058,7 @@
       <c r="F30" t="s">
         <v>533</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="4">
         <v>45980</v>
       </c>
       <c r="J30">
@@ -9638,7 +10093,7 @@
       <c r="F31" t="s">
         <v>536</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="4">
         <v>45980</v>
       </c>
       <c r="J31">
@@ -9673,7 +10128,7 @@
       <c r="F32" t="s">
         <v>539</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="4">
         <v>45980</v>
       </c>
       <c r="J32">
@@ -9708,7 +10163,7 @@
       <c r="F33" t="s">
         <v>542</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="4">
         <v>45980</v>
       </c>
       <c r="J33">
@@ -9743,7 +10198,7 @@
       <c r="F34" t="s">
         <v>545</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="4">
         <v>45980</v>
       </c>
       <c r="J34">
@@ -9778,7 +10233,7 @@
       <c r="F35" t="s">
         <v>548</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="4">
         <v>45980</v>
       </c>
       <c r="J35">
@@ -9813,7 +10268,7 @@
       <c r="F36" t="s">
         <v>551</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="4">
         <v>45980</v>
       </c>
       <c r="J36">
@@ -9848,7 +10303,7 @@
       <c r="F37" t="s">
         <v>554</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="4">
         <v>45980</v>
       </c>
       <c r="J37">
@@ -9883,7 +10338,7 @@
       <c r="F38" t="s">
         <v>557</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="4">
         <v>45980</v>
       </c>
       <c r="J38">
@@ -9918,7 +10373,7 @@
       <c r="F39" t="s">
         <v>560</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="4">
         <v>45980</v>
       </c>
       <c r="J39">
@@ -9953,7 +10408,7 @@
       <c r="F40" t="s">
         <v>563</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="4">
         <v>45980</v>
       </c>
       <c r="J40">
@@ -9988,7 +10443,7 @@
       <c r="F41" t="s">
         <v>566</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="4">
         <v>45980</v>
       </c>
       <c r="J41">
@@ -10023,7 +10478,7 @@
       <c r="F42" t="s">
         <v>569</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="4">
         <v>45980</v>
       </c>
       <c r="J42">
@@ -10058,7 +10513,7 @@
       <c r="F43" t="s">
         <v>572</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="4">
         <v>45980</v>
       </c>
       <c r="J43">
@@ -10093,7 +10548,7 @@
       <c r="F44" t="s">
         <v>575</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="4">
         <v>45980</v>
       </c>
       <c r="J44">
@@ -10128,7 +10583,7 @@
       <c r="F45" t="s">
         <v>578</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="4">
         <v>45980</v>
       </c>
       <c r="J45">
@@ -10163,7 +10618,7 @@
       <c r="F46" t="s">
         <v>581</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="4">
         <v>45980</v>
       </c>
       <c r="J46">
@@ -10198,7 +10653,7 @@
       <c r="F47" t="s">
         <v>584</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="4">
         <v>45980</v>
       </c>
       <c r="J47">
@@ -10233,7 +10688,7 @@
       <c r="F48" t="s">
         <v>587</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="4">
         <v>45980</v>
       </c>
       <c r="J48">
@@ -10268,7 +10723,7 @@
       <c r="F49" t="s">
         <v>590</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="4">
         <v>45980</v>
       </c>
       <c r="J49">
@@ -10303,7 +10758,7 @@
       <c r="F50" t="s">
         <v>593</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="4">
         <v>45980</v>
       </c>
       <c r="J50">
@@ -10338,7 +10793,7 @@
       <c r="F51" t="s">
         <v>596</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="4">
         <v>45980</v>
       </c>
       <c r="J51">
@@ -10373,7 +10828,7 @@
       <c r="F52" t="s">
         <v>599</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="4">
         <v>45980</v>
       </c>
       <c r="J52">
@@ -10408,7 +10863,7 @@
       <c r="F53" t="s">
         <v>602</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="4">
         <v>45980</v>
       </c>
       <c r="J53">
@@ -10443,7 +10898,7 @@
       <c r="F54" t="s">
         <v>605</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="4">
         <v>45980</v>
       </c>
       <c r="J54">
@@ -10478,7 +10933,7 @@
       <c r="F55" t="s">
         <v>608</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55" s="4">
         <v>45980</v>
       </c>
       <c r="J55">
@@ -10513,7 +10968,7 @@
       <c r="F56" t="s">
         <v>611</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="4">
         <v>45980</v>
       </c>
       <c r="J56">
@@ -10548,7 +11003,7 @@
       <c r="F57" t="s">
         <v>614</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57" s="4">
         <v>45980</v>
       </c>
       <c r="J57">
@@ -10583,7 +11038,7 @@
       <c r="F58" t="s">
         <v>617</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H58" s="4">
         <v>45980</v>
       </c>
       <c r="J58">
@@ -10618,7 +11073,7 @@
       <c r="F59" t="s">
         <v>620</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="4">
         <v>45980</v>
       </c>
       <c r="J59">
@@ -10653,7 +11108,7 @@
       <c r="F60" t="s">
         <v>623</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="4">
         <v>45980</v>
       </c>
       <c r="J60">
@@ -10688,7 +11143,7 @@
       <c r="F61" t="s">
         <v>626</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H61" s="4">
         <v>45980</v>
       </c>
       <c r="J61">
@@ -10723,7 +11178,7 @@
       <c r="F62" t="s">
         <v>629</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H62" s="4">
         <v>45980</v>
       </c>
       <c r="J62">
@@ -10758,7 +11213,7 @@
       <c r="F63" t="s">
         <v>632</v>
       </c>
-      <c r="H63" s="3">
+      <c r="H63" s="4">
         <v>45980</v>
       </c>
       <c r="J63">
@@ -10793,7 +11248,7 @@
       <c r="F64" t="s">
         <v>635</v>
       </c>
-      <c r="H64" s="3">
+      <c r="H64" s="4">
         <v>45980</v>
       </c>
       <c r="J64">
@@ -12309,8 +12764,8 @@
   <sheetPr/>
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -12436,7 +12891,7 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>45982</v>
       </c>
       <c r="J6">
@@ -12474,7 +12929,7 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>45982</v>
       </c>
       <c r="J7">
@@ -12512,7 +12967,7 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>45982</v>
       </c>
       <c r="J8">
@@ -12550,7 +13005,7 @@
       <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>45982</v>
       </c>
       <c r="J9">
@@ -12588,7 +13043,7 @@
       <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>45982</v>
       </c>
       <c r="J10">
@@ -12626,7 +13081,7 @@
       <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>45982</v>
       </c>
       <c r="J11">
@@ -12664,7 +13119,7 @@
       <c r="G12" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>45982</v>
       </c>
       <c r="J12">
@@ -12702,7 +13157,7 @@
       <c r="G13" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>45982</v>
       </c>
       <c r="J13">
@@ -12740,7 +13195,7 @@
       <c r="G14" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>45982</v>
       </c>
       <c r="J14">
@@ -12778,7 +13233,7 @@
       <c r="G15" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>45982</v>
       </c>
       <c r="J15">
@@ -12816,7 +13271,7 @@
       <c r="G16" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>45982</v>
       </c>
       <c r="J16">
@@ -12854,7 +13309,7 @@
       <c r="G17" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>45982</v>
       </c>
       <c r="J17">
@@ -12892,7 +13347,7 @@
       <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>45982</v>
       </c>
       <c r="J18">
@@ -12930,7 +13385,7 @@
       <c r="G19" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>45982</v>
       </c>
       <c r="J19">
@@ -12968,7 +13423,7 @@
       <c r="G20" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>45982</v>
       </c>
       <c r="J20">
@@ -13006,7 +13461,7 @@
       <c r="G21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>45982</v>
       </c>
       <c r="J21">
@@ -13047,7 +13502,7 @@
       <c r="H22" t="s">
         <v>760</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -13085,7 +13540,7 @@
       <c r="H23" t="s">
         <v>760</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -13123,7 +13578,7 @@
       <c r="H24" t="s">
         <v>760</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -13158,7 +13613,7 @@
       <c r="G25" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>45982</v>
       </c>
       <c r="J25">
@@ -13196,7 +13651,7 @@
       <c r="G26" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>45982</v>
       </c>
       <c r="J26">
@@ -13234,7 +13689,7 @@
       <c r="G27" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>45982</v>
       </c>
       <c r="J27">
@@ -13272,7 +13727,7 @@
       <c r="G28" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>45982</v>
       </c>
       <c r="J28">
@@ -13310,7 +13765,7 @@
       <c r="G29" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="4">
         <v>45982</v>
       </c>
       <c r="J29">
@@ -13348,7 +13803,7 @@
       <c r="G30" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="4">
         <v>45982</v>
       </c>
       <c r="J30">
@@ -13389,7 +13844,7 @@
       <c r="H31" t="s">
         <v>760</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -13424,7 +13879,7 @@
       <c r="G32" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="4">
         <v>45982</v>
       </c>
       <c r="J32">
@@ -13462,7 +13917,7 @@
       <c r="G33" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="4">
         <v>45982</v>
       </c>
       <c r="J33">
@@ -13500,7 +13955,7 @@
       <c r="G34" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="4">
         <v>45982</v>
       </c>
       <c r="J34">
@@ -13541,7 +13996,7 @@
       <c r="H35" t="s">
         <v>760</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
@@ -13579,7 +14034,7 @@
       <c r="H36" t="s">
         <v>760</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
@@ -13614,7 +14069,7 @@
       <c r="G37" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="4">
         <v>45982</v>
       </c>
       <c r="J37">
@@ -13652,7 +14107,7 @@
       <c r="G38" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="4">
         <v>45982</v>
       </c>
       <c r="J38">
@@ -13690,7 +14145,7 @@
       <c r="G39" t="s">
         <v>863</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="4">
         <v>45982</v>
       </c>
       <c r="J39">
@@ -13728,7 +14183,7 @@
       <c r="G40" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="4">
         <v>45982</v>
       </c>
       <c r="J40">
@@ -13766,7 +14221,7 @@
       <c r="G41" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="4">
         <v>45982</v>
       </c>
       <c r="J41">
@@ -13804,7 +14259,7 @@
       <c r="G42" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="4">
         <v>45982</v>
       </c>
       <c r="J42">
@@ -13842,7 +14297,7 @@
       <c r="G43" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="4">
         <v>45982</v>
       </c>
       <c r="J43">
@@ -13880,7 +14335,7 @@
       <c r="G44" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="4">
         <v>45982</v>
       </c>
       <c r="J44">
@@ -13921,7 +14376,7 @@
       <c r="H45" t="s">
         <v>760</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
@@ -13959,7 +14414,7 @@
       <c r="H46" t="s">
         <v>760</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="3">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -13982,4 +14437,1801 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.57142857142857" customWidth="1"/>
+    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="16.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="29.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="4.71428571428571" customWidth="1"/>
+    <col min="6" max="6" width="15.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="32.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="16.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="6.57142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>22862</v>
+      </c>
+      <c r="C5" t="s">
+        <v>886</v>
+      </c>
+      <c r="D5" t="s">
+        <v>887</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>888</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <f>A5</f>
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
+        <f>F5</f>
+        <v>085263362906</v>
+      </c>
+      <c r="L5" t="str">
+        <f>D5</f>
+        <v>ADISTO PRASATYO</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>22863</v>
+      </c>
+      <c r="C6" t="s">
+        <v>889</v>
+      </c>
+      <c r="D6" t="s">
+        <v>890</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>891</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J53" si="0">A6</f>
+        <v>2</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K53" si="1">F6</f>
+        <v>08126876989</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L53" si="2">D6</f>
+        <v>AGUS HERI SANTOSO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>22864</v>
+      </c>
+      <c r="C7" t="s">
+        <v>892</v>
+      </c>
+      <c r="D7" t="s">
+        <v>893</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>894</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>085374291252</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>ALFIAN</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>22865</v>
+      </c>
+      <c r="C8" t="s">
+        <v>895</v>
+      </c>
+      <c r="D8" t="s">
+        <v>896</v>
+      </c>
+      <c r="E8">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>897</v>
+      </c>
+      <c r="G8" t="s">
+        <v>898</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>081266055292</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>AMIZAR ZULMI NASUTION</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>22866</v>
+      </c>
+      <c r="C9" t="s">
+        <v>899</v>
+      </c>
+      <c r="D9" t="s">
+        <v>900</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>901</v>
+      </c>
+      <c r="G9" t="s">
+        <v>898</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>082283149719</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>ANDIKA BATRA SUKARYA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>22867</v>
+      </c>
+      <c r="C10" t="s">
+        <v>902</v>
+      </c>
+      <c r="D10" t="s">
+        <v>903</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>904</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>083892354614</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>ANDIKA PAMUNGKAS</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>22868</v>
+      </c>
+      <c r="C11" t="s">
+        <v>905</v>
+      </c>
+      <c r="D11" t="s">
+        <v>906</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>907</v>
+      </c>
+      <c r="G11" t="s">
+        <v>898</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>083188852207</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>ANGGA ARDIANSYAH</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>22869</v>
+      </c>
+      <c r="C12" t="s">
+        <v>908</v>
+      </c>
+      <c r="D12" t="s">
+        <v>909</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>910</v>
+      </c>
+      <c r="G12" t="s">
+        <v>898</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>0895400640694</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>ANGGA WIDI SYAHPUTRA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>22870</v>
+      </c>
+      <c r="C13" t="s">
+        <v>911</v>
+      </c>
+      <c r="D13" t="s">
+        <v>912</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>913</v>
+      </c>
+      <c r="G13" t="s">
+        <v>898</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>085356301551</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>AZWALI KHAIRI</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>22871</v>
+      </c>
+      <c r="C14" t="s">
+        <v>914</v>
+      </c>
+      <c r="D14" t="s">
+        <v>915</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>916</v>
+      </c>
+      <c r="G14" t="s">
+        <v>898</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>085765279425</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>BASARI</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>22872</v>
+      </c>
+      <c r="C15" t="s">
+        <v>917</v>
+      </c>
+      <c r="D15" t="s">
+        <v>918</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>919</v>
+      </c>
+      <c r="G15" t="s">
+        <v>898</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>082247069508</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>CANDRA MUDA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>22873</v>
+      </c>
+      <c r="C16" t="s">
+        <v>920</v>
+      </c>
+      <c r="D16" t="s">
+        <v>921</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>922</v>
+      </c>
+      <c r="G16" t="s">
+        <v>898</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>081374446609</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>DAFIT HELDI</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>22874</v>
+      </c>
+      <c r="C17" t="s">
+        <v>923</v>
+      </c>
+      <c r="D17" t="s">
+        <v>924</v>
+      </c>
+      <c r="E17">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>925</v>
+      </c>
+      <c r="G17" t="s">
+        <v>898</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>081223853171</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>EPI KARINA</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>22875</v>
+      </c>
+      <c r="C18" t="s">
+        <v>926</v>
+      </c>
+      <c r="D18" t="s">
+        <v>927</v>
+      </c>
+      <c r="E18">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>928</v>
+      </c>
+      <c r="G18" t="s">
+        <v>898</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>082384226483</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>ESTER BR PARDEDE</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>22876</v>
+      </c>
+      <c r="C19" t="s">
+        <v>929</v>
+      </c>
+      <c r="D19" t="s">
+        <v>930</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>931</v>
+      </c>
+      <c r="G19" t="s">
+        <v>932</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>087845627099</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>FERTO ATAUPAH</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>22877</v>
+      </c>
+      <c r="C20" t="s">
+        <v>933</v>
+      </c>
+      <c r="D20" t="s">
+        <v>934</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>935</v>
+      </c>
+      <c r="G20" t="s">
+        <v>898</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>082171582482</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>GUSTI JUPRI ANDA MAULANA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>22878</v>
+      </c>
+      <c r="C21" t="s">
+        <v>936</v>
+      </c>
+      <c r="D21" t="s">
+        <v>937</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>938</v>
+      </c>
+      <c r="G21" t="s">
+        <v>898</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>088708395531</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>HEBRA LENDI</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>22879</v>
+      </c>
+      <c r="C22" t="s">
+        <v>939</v>
+      </c>
+      <c r="D22" t="s">
+        <v>940</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>941</v>
+      </c>
+      <c r="G22" t="s">
+        <v>898</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>085717412709</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>HENI FARIDA</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>22880</v>
+      </c>
+      <c r="C23" t="s">
+        <v>942</v>
+      </c>
+      <c r="D23" t="s">
+        <v>943</v>
+      </c>
+      <c r="E23">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>944</v>
+      </c>
+      <c r="G23" t="s">
+        <v>898</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>087714822536</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="2"/>
+        <v>HERI PRATAMA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>22881</v>
+      </c>
+      <c r="C24" t="s">
+        <v>945</v>
+      </c>
+      <c r="D24" t="s">
+        <v>946</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>947</v>
+      </c>
+      <c r="G24" t="s">
+        <v>898</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>081350740931</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="2"/>
+        <v>HERY JUNIANTO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>22882</v>
+      </c>
+      <c r="C25" t="s">
+        <v>948</v>
+      </c>
+      <c r="D25" t="s">
+        <v>949</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>950</v>
+      </c>
+      <c r="G25" t="s">
+        <v>898</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>085831045258</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="2"/>
+        <v>IRA TRISULA ARDYANTI</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>22883</v>
+      </c>
+      <c r="C26" t="s">
+        <v>951</v>
+      </c>
+      <c r="D26" t="s">
+        <v>677</v>
+      </c>
+      <c r="E26">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>952</v>
+      </c>
+      <c r="G26" t="s">
+        <v>898</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>087784857563</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="2"/>
+        <v>ISKANDAR</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>22884</v>
+      </c>
+      <c r="C27" t="s">
+        <v>953</v>
+      </c>
+      <c r="D27" t="s">
+        <v>954</v>
+      </c>
+      <c r="E27">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s">
+        <v>955</v>
+      </c>
+      <c r="G27" t="s">
+        <v>898</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>083838917190</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="2"/>
+        <v>ISMAIL</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>22885</v>
+      </c>
+      <c r="C28" t="s">
+        <v>956</v>
+      </c>
+      <c r="D28" t="s">
+        <v>957</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+      <c r="F28" t="s">
+        <v>958</v>
+      </c>
+      <c r="G28" t="s">
+        <v>898</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>081270074533</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="2"/>
+        <v>JAPRI</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>22886</v>
+      </c>
+      <c r="C29" t="s">
+        <v>959</v>
+      </c>
+      <c r="D29" t="s">
+        <v>960</v>
+      </c>
+      <c r="E29">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>961</v>
+      </c>
+      <c r="G29" t="s">
+        <v>898</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>082177252459</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="2"/>
+        <v>JUPRIANTO</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>22887</v>
+      </c>
+      <c r="C30" t="s">
+        <v>962</v>
+      </c>
+      <c r="D30" t="s">
+        <v>963</v>
+      </c>
+      <c r="E30">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>964</v>
+      </c>
+      <c r="G30" t="s">
+        <v>898</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>083809783587</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="2"/>
+        <v>LAURA SYAFIKHA PUTRI</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>22888</v>
+      </c>
+      <c r="C31" t="s">
+        <v>965</v>
+      </c>
+      <c r="D31" t="s">
+        <v>966</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>967</v>
+      </c>
+      <c r="G31" t="s">
+        <v>898</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>082122082309</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="2"/>
+        <v>LESMAN LUMBANTORUAN</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>22889</v>
+      </c>
+      <c r="C32" t="s">
+        <v>968</v>
+      </c>
+      <c r="D32" t="s">
+        <v>969</v>
+      </c>
+      <c r="E32">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>970</v>
+      </c>
+      <c r="G32" t="s">
+        <v>971</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>082286941927</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="2"/>
+        <v>LUHUT SITUMORANG</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>22890</v>
+      </c>
+      <c r="C33" t="s">
+        <v>972</v>
+      </c>
+      <c r="D33" t="s">
+        <v>973</v>
+      </c>
+      <c r="E33">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>974</v>
+      </c>
+      <c r="G33" t="s">
+        <v>975</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>085809836590</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="2"/>
+        <v>MARDIAH</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>22891</v>
+      </c>
+      <c r="C34" t="s">
+        <v>976</v>
+      </c>
+      <c r="D34" t="s">
+        <v>977</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>978</v>
+      </c>
+      <c r="G34" t="s">
+        <v>898</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>083835723800</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="2"/>
+        <v>MUHAMMAD BUDI</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>22892</v>
+      </c>
+      <c r="C35" t="s">
+        <v>979</v>
+      </c>
+      <c r="D35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>981</v>
+      </c>
+      <c r="G35" t="s">
+        <v>898</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>089668459090</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="2"/>
+        <v>MUHAMMAD HARIYANTO</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>22893</v>
+      </c>
+      <c r="C36" t="s">
+        <v>982</v>
+      </c>
+      <c r="D36" t="s">
+        <v>983</v>
+      </c>
+      <c r="E36">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>984</v>
+      </c>
+      <c r="G36" t="s">
+        <v>971</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>082339861630</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="2"/>
+        <v>MUHAMMAD JUNAIDI</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>22894</v>
+      </c>
+      <c r="C37" t="s">
+        <v>985</v>
+      </c>
+      <c r="D37" t="s">
+        <v>986</v>
+      </c>
+      <c r="E37">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>987</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="1"/>
+        <v>081364059451</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="2"/>
+        <v>MUJI HARYANTO</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>22895</v>
+      </c>
+      <c r="C38" t="s">
+        <v>988</v>
+      </c>
+      <c r="D38" t="s">
+        <v>989</v>
+      </c>
+      <c r="E38">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s">
+        <v>990</v>
+      </c>
+      <c r="G38" t="s">
+        <v>898</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="1"/>
+        <v>082287796354</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="2"/>
+        <v>MUSLIMIN</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>22896</v>
+      </c>
+      <c r="C39" t="s">
+        <v>991</v>
+      </c>
+      <c r="D39" t="s">
+        <v>992</v>
+      </c>
+      <c r="E39">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>993</v>
+      </c>
+      <c r="G39" t="s">
+        <v>898</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="1"/>
+        <v>082214594160</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="2"/>
+        <v>NOVEDI LAOLI</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>22897</v>
+      </c>
+      <c r="C40" t="s">
+        <v>994</v>
+      </c>
+      <c r="D40" t="s">
+        <v>995</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>996</v>
+      </c>
+      <c r="G40" t="s">
+        <v>898</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="1"/>
+        <v>082294790044</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="2"/>
+        <v>POSMARITO NDRAHA</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>22898</v>
+      </c>
+      <c r="C41" t="s">
+        <v>997</v>
+      </c>
+      <c r="D41" t="s">
+        <v>998</v>
+      </c>
+      <c r="E41">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>999</v>
+      </c>
+      <c r="G41" t="s">
+        <v>898</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="1"/>
+        <v>085769897824</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="2"/>
+        <v>RAFI RIZKY SYAHPUTRA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>22899</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G42" t="s">
+        <v>898</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="1"/>
+        <v>088271719392</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="2"/>
+        <v>RAHEL ANDRIANSYAH</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>22900</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E43">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1005</v>
+      </c>
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="1"/>
+        <v>082172430974</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="2"/>
+        <v>RIA SUHARTI</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>22901</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E44">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G44" t="s">
+        <v>898</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="1"/>
+        <v>082386778113</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="2"/>
+        <v>RIAN ANGGARA SAPUTRA</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>22902</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E45">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G45" t="s">
+        <v>898</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="1"/>
+        <v>081266670060</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="2"/>
+        <v>RIDWAN</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>22903</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E46">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G46" t="s">
+        <v>898</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="1"/>
+        <v>087877303641</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="2"/>
+        <v>RINA SRI DEWI</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>22904</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E47">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G47" t="s">
+        <v>898</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="1"/>
+        <v>6281374154280</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="2"/>
+        <v>TARMIZI</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>22905</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E48">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G48" t="s">
+        <v>898</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="1"/>
+        <v>085185741050</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="2"/>
+        <v>TUMINI</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>22906</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E49">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G49" t="s">
+        <v>898</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="1"/>
+        <v>081277441909</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="2"/>
+        <v>USMAN HADINATHA</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>22907</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E50">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G50" t="s">
+        <v>898</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="1"/>
+        <v>082351191910</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="2"/>
+        <v>WENDRI</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>22908</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E51">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" s="3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="1"/>
+        <v>081365214431</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="2"/>
+        <v>YANTI</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>22909</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E52">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G52" t="s">
+        <v>898</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="1"/>
+        <v>081371952939</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="2"/>
+        <v>YUNITA HANDAYANI</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>22910</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E53">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G53" t="s">
+        <v>971</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="1"/>
+        <v>083824710553</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="2"/>
+        <v>ZATIAWATI</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A5:H53">
+    <sortCondition ref="D6"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>